<commit_message>
Update the number of pieces of Cost4
</commit_message>
<xml_diff>
--- a/Data/Probability Chart_season_10.xlsx
+++ b/Data/Probability Chart_season_10.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11295"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11295" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Probability Cost" sheetId="1" r:id="rId1"/>
@@ -364,7 +364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -637,10 +637,10 @@
         <v>18</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update the number of pieces for each costs
</commit_message>
<xml_diff>
--- a/Data/Probability Chart_season_10.xlsx
+++ b/Data/Probability Chart_season_10.xlsx
@@ -598,7 +598,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -628,13 +628,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>10</v>

</xml_diff>

<commit_message>
Update Season10 Prob_champbag & Comps recomendation
</commit_message>
<xml_diff>
--- a/Data/Probability Chart_season_10.xlsx
+++ b/Data/Probability Chart_season_10.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\TFT_Probability_Streamlit\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snow/Desktop/PyProjects/TFT_Probability_Streamlit/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EC2BDA-2420-2542-86F6-69430E0BFE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11295" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25120" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Probability Cost" sheetId="1" r:id="rId1"/>
@@ -38,8 +39,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,16 +362,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="B1">
         <v>1</v>
       </c>
@@ -387,7 +388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -407,7 +408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -427,7 +428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -447,7 +448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -467,7 +468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -487,18 +488,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="C7">
         <v>0.4</v>
       </c>
       <c r="D7">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E7">
         <v>0.05</v>
@@ -507,7 +508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -515,10 +516,10 @@
         <v>0.19</v>
       </c>
       <c r="C8">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="D8">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="E8">
         <v>0.1</v>
@@ -527,7 +528,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -547,7 +548,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -555,10 +556,10 @@
         <v>0.1</v>
       </c>
       <c r="C10">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D10">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="E10">
         <v>0.35</v>
@@ -567,7 +568,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -594,19 +595,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="B1">
         <v>1</v>
       </c>
@@ -623,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -643,7 +644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>

</xml_diff>